<commit_message>
bug fixes,  all works well
gamcreate works well, excelgreep works ok, gamcreate searches all excel files
</commit_message>
<xml_diff>
--- a/codes.xlsx
+++ b/codes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byates\OneDrive - Roswell Independent School District\Documents\GitHub\gamCreate4Chromebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{8DCFCB8D-105D-49C8-9CB4-3FF0CC0E947C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{9D1D0A40-9968-41C3-AEE8-21FCEC568FB4}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{8DCFCB8D-105D-49C8-9CB4-3FF0CC0E947C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D194E499-674F-42E3-9116-07CB4E09CC83}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{E05A1B20-41DA-48C0-BE76-3A13FD40B8EE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
   <si>
     <t>SUN</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>/ADMIN</t>
-  </si>
-  <si>
-    <t>Target OU (created if needed)</t>
   </si>
   <si>
     <t>School</t>
@@ -181,9 +178,6 @@
     <t>NOTecarr@risd.k12.nm.us</t>
   </si>
   <si>
-    <t>SMS Cart 15 2021</t>
-  </si>
-  <si>
     <t>NOTbgreen@risd.k12.nm.us</t>
   </si>
   <si>
@@ -196,16 +190,22 @@
     <t>NOTechapman@risd.k12.nm.us</t>
   </si>
   <si>
-    <t>jsoltero@risd.k12.nm.us</t>
-  </si>
-  <si>
-    <t>/STUDENTS/ELEMENTARY/NLE/NLE Cart 2 2021</t>
-  </si>
-  <si>
-    <t>Cart 2 2021</t>
-  </si>
-  <si>
     <t>/STUDENTS/ELEMENTARY/PEC</t>
+  </si>
+  <si>
+    <t>NOTjsoltero@risd.k12.nm.us</t>
+  </si>
+  <si>
+    <t>Target OU (created if needed) (NEW EACH TIME)</t>
+  </si>
+  <si>
+    <t>/STUDENTS/ELEMENTARY/NLE/</t>
+  </si>
+  <si>
+    <t>ecarr@risd.k12.nm.us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BES Cart 4 2021 </t>
   </si>
 </sst>
 </file>
@@ -620,7 +620,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,13 +635,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
       </c>
       <c r="D1" t="s">
         <v>33</v>
@@ -653,7 +653,7 @@
         <v>36</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -665,7 +665,7 @@
       </c>
       <c r="C2" s="1"/>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" s="7"/>
     </row>
@@ -675,12 +675,14 @@
       </c>
       <c r="B3" t="str">
         <f>"/STUDENTS/ELEMENTARY/BES/"&amp;D3</f>
-        <v>/STUDENTS/ELEMENTARY/BES/</v>
+        <v xml:space="preserve">/STUDENTS/ELEMENTARY/BES/BES Cart 4 2021 </v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
@@ -709,7 +711,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
         <v>34</v>
@@ -724,7 +726,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
@@ -739,11 +741,9 @@
         <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>58</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D7" s="6"/>
       <c r="E7" t="s">
         <v>9</v>
       </c>
@@ -769,10 +769,10 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
@@ -811,10 +811,10 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
         <v>34</v>
@@ -829,7 +829,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
@@ -857,7 +857,7 @@
         <v>/STUDENTS/MIDDLE/BMS/</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
@@ -898,14 +898,12 @@
       </c>
       <c r="B18" t="str">
         <f>"/STUDENTS/MIDDLE/SMS/"&amp;D18</f>
-        <v>/STUDENTS/MIDDLE/SMS/SMS Cart 15 2021</v>
+        <v>/STUDENTS/MIDDLE/SMS/</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>51</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D18" s="5"/>
       <c r="E18" t="s">
         <v>13</v>
       </c>
@@ -985,14 +983,14 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G1:G22"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F23" xr:uid="{3CA40D1C-9639-4BC9-8E26-59271DC4B632}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>

</xml_diff>